<commit_message>
Routing and gerber files produced
</commit_message>
<xml_diff>
--- a/2022_02_11_LED_Driver_PCB/Project Outputs for 2022_02_11_LED_Driver_PCB/2022_02_11_LED_Driver_PCB.xlsx
+++ b/2022_02_11_LED_Driver_PCB/Project Outputs for 2022_02_11_LED_Driver_PCB/2022_02_11_LED_Driver_PCB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\javi_\GitHub\LED_Driver_Deco\2022_02_11_LED_Driver_PCB\Project Outputs for 2022_02_11_LED_Driver_PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AFF52347-B005-4B73-976B-A344BD46D3C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D7ABE4E0-E7A9-428F-9A67-7339FA3ABB11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17850" yWindow="2865" windowWidth="10950" windowHeight="12735" xr2:uid="{4A41DCB0-F543-4467-8352-47615947B6C8}"/>
+    <workbookView xWindow="17850" yWindow="2865" windowWidth="10950" windowHeight="12735" xr2:uid="{E2144E6A-6BAB-415C-993E-3E25E62760E3}"/>
   </bookViews>
   <sheets>
     <sheet name="2022_02_11_LED_Driver_PCB" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="59">
   <si>
     <t>Description</t>
   </si>
@@ -64,7 +64,7 @@
     <t>C0805C104K5RAC7411</t>
   </si>
   <si>
-    <t>C1, C2, C5, C6, C9</t>
+    <t>C1, C2, C3, C6, C7, C10, C11</t>
   </si>
   <si>
     <t>CAPC2012X94N</t>
@@ -73,18 +73,30 @@
     <t>08055A4R3CAT2A</t>
   </si>
   <si>
-    <t>C3, C4</t>
+    <t>C4, C5</t>
   </si>
   <si>
     <t>885012107015</t>
   </si>
   <si>
-    <t>C7, C8</t>
+    <t>C8, C9</t>
   </si>
   <si>
     <t>CAPC2012X135N</t>
   </si>
   <si>
+    <t>USB connector</t>
+  </si>
+  <si>
+    <t>920-E52A2021S10100</t>
+  </si>
+  <si>
+    <t>CN1</t>
+  </si>
+  <si>
+    <t>USB307530A</t>
+  </si>
+  <si>
     <t>Integrated Circuit</t>
   </si>
   <si>
@@ -116,6 +128,24 @@
   </si>
   <si>
     <t>SOIC127P600X175-9N</t>
+  </si>
+  <si>
+    <t>Connector</t>
+  </si>
+  <si>
+    <t>4PIN</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>B2B-PH-K-S_LF__SN_</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>SHDR2W50P0X200_1X2_590X450X600P</t>
   </si>
   <si>
     <t>Inductor</t>
@@ -560,8 +590,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E67B7EB-95BA-4E7A-A72B-2C74CC3CFDC8}">
-  <dimension ref="A1:F14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5D5E5F2-9690-4F94-9E1C-248B9E92DC77}">
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -609,7 +639,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -694,19 +724,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="F7" s="1">
         <v>1</v>
@@ -714,7 +744,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>27</v>
@@ -743,7 +773,7 @@
         <v>32</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>31</v>
@@ -754,19 +784,19 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="E10" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F10" s="1">
         <v>1</v>
@@ -774,7 +804,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>37</v>
@@ -783,7 +813,7 @@
         <v>38</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>37</v>
@@ -794,39 +824,39 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="F12" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F13" s="1">
         <v>1</v>
@@ -834,21 +864,81 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="F14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>